<commit_message>
Add Automi AI project with Power BI setup, ARL energy analysis, and UGE_LVMT automation project
</commit_message>
<xml_diff>
--- a/asseco_data_systems/asseco_scraped_data.xlsx
+++ b/asseco_data_systems/asseco_scraped_data.xlsx
@@ -507,7 +507,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H2" t="n">
@@ -545,7 +545,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H3" t="n">
@@ -583,7 +583,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H4" t="n">
@@ -621,7 +621,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H5" t="n">
@@ -659,7 +659,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H6" t="n">
@@ -697,7 +697,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H7" t="n">
@@ -735,7 +735,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H8" t="n">
@@ -773,7 +773,7 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H9" t="n">
@@ -811,7 +811,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H10" t="n">
@@ -849,7 +849,7 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H11" t="n">
@@ -887,7 +887,7 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H12" t="n">
@@ -925,7 +925,7 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H13" t="n">
@@ -963,7 +963,7 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H14" t="n">
@@ -1001,7 +1001,7 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H15" t="n">
@@ -1039,7 +1039,7 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H16" t="n">
@@ -1077,7 +1077,7 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H17" t="n">
@@ -1115,7 +1115,7 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H18" t="n">
@@ -1153,7 +1153,7 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H19" t="n">
@@ -1191,7 +1191,7 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H20" t="n">
@@ -1229,7 +1229,7 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H21" t="n">
@@ -1267,7 +1267,7 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H22" t="n">
@@ -1305,7 +1305,7 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H23" t="n">
@@ -1343,7 +1343,7 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H24" t="n">
@@ -1381,7 +1381,7 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H25" t="n">
@@ -1419,7 +1419,7 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H26" t="n">
@@ -1457,7 +1457,7 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H27" t="n">
@@ -1495,7 +1495,7 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H28" t="n">
@@ -1533,7 +1533,7 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H29" t="n">
@@ -1571,7 +1571,7 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H30" t="n">
@@ -1609,7 +1609,7 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H31" t="n">
@@ -1647,7 +1647,7 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H32" t="n">
@@ -1685,7 +1685,7 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H33" t="n">
@@ -1723,7 +1723,7 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H34" t="n">
@@ -1761,7 +1761,7 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H35" t="n">
@@ -1799,7 +1799,7 @@
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H36" t="n">
@@ -1837,7 +1837,7 @@
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H37" t="n">
@@ -1875,7 +1875,7 @@
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H38" t="n">
@@ -1913,7 +1913,7 @@
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H39" t="n">
@@ -1951,7 +1951,7 @@
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H40" t="n">
@@ -1989,7 +1989,7 @@
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H41" t="n">
@@ -2027,7 +2027,7 @@
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H42" t="n">
@@ -2065,7 +2065,7 @@
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H43" t="n">
@@ -2103,7 +2103,7 @@
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H44" t="n">
@@ -2141,7 +2141,7 @@
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H45" t="n">
@@ -2179,7 +2179,7 @@
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H46" t="n">
@@ -2217,7 +2217,7 @@
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H47" t="n">
@@ -2255,7 +2255,7 @@
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H48" t="n">
@@ -2293,7 +2293,7 @@
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H49" t="n">
@@ -2331,7 +2331,7 @@
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H50" t="n">
@@ -2369,7 +2369,7 @@
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H51" t="n">
@@ -2407,7 +2407,7 @@
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H52" t="n">
@@ -2445,7 +2445,7 @@
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H53" t="n">
@@ -2483,7 +2483,7 @@
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H54" t="n">
@@ -2521,7 +2521,7 @@
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H55" t="n">
@@ -2559,7 +2559,7 @@
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H56" t="n">
@@ -2597,7 +2597,7 @@
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H57" t="n">
@@ -2635,7 +2635,7 @@
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H58" t="n">
@@ -2673,7 +2673,7 @@
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H59" t="n">
@@ -2711,7 +2711,7 @@
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H60" t="n">
@@ -2749,7 +2749,7 @@
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H61" t="n">
@@ -2787,7 +2787,7 @@
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H62" t="n">
@@ -2825,7 +2825,7 @@
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H63" t="n">
@@ -2863,7 +2863,7 @@
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H64" t="n">
@@ -2901,7 +2901,7 @@
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H65" t="n">
@@ -2939,7 +2939,7 @@
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H66" t="n">
@@ -2977,7 +2977,7 @@
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H67" t="n">
@@ -3015,7 +3015,7 @@
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H68" t="n">
@@ -3053,7 +3053,7 @@
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H69" t="n">
@@ -3091,7 +3091,7 @@
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H70" t="n">
@@ -3129,7 +3129,7 @@
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H71" t="n">
@@ -3167,7 +3167,7 @@
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H72" t="n">
@@ -3205,7 +3205,7 @@
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H73" t="n">
@@ -3243,7 +3243,7 @@
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H74" t="n">
@@ -3281,7 +3281,7 @@
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H75" t="n">
@@ -3319,7 +3319,7 @@
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H76" t="n">
@@ -3357,7 +3357,7 @@
       </c>
       <c r="G77" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H77" t="n">
@@ -3395,7 +3395,7 @@
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H78" t="n">
@@ -3433,7 +3433,7 @@
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H79" t="n">
@@ -3471,7 +3471,7 @@
       </c>
       <c r="G80" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H80" t="n">
@@ -3509,7 +3509,7 @@
       </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H81" t="n">
@@ -3547,7 +3547,7 @@
       </c>
       <c r="G82" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H82" t="n">
@@ -3585,7 +3585,7 @@
       </c>
       <c r="G83" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H83" t="n">
@@ -3623,7 +3623,7 @@
       </c>
       <c r="G84" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H84" t="n">
@@ -3661,7 +3661,7 @@
       </c>
       <c r="G85" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H85" t="n">
@@ -3699,7 +3699,7 @@
       </c>
       <c r="G86" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H86" t="n">
@@ -3737,7 +3737,7 @@
       </c>
       <c r="G87" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H87" t="n">
@@ -3775,7 +3775,7 @@
       </c>
       <c r="G88" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H88" t="n">
@@ -3813,7 +3813,7 @@
       </c>
       <c r="G89" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H89" t="n">
@@ -3851,7 +3851,7 @@
       </c>
       <c r="G90" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H90" t="n">
@@ -3889,7 +3889,7 @@
       </c>
       <c r="G91" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H91" t="n">
@@ -3927,7 +3927,7 @@
       </c>
       <c r="G92" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H92" t="n">
@@ -3965,7 +3965,7 @@
       </c>
       <c r="G93" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H93" t="n">
@@ -4003,7 +4003,7 @@
       </c>
       <c r="G94" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H94" t="n">
@@ -4041,7 +4041,7 @@
       </c>
       <c r="G95" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H95" t="n">
@@ -4079,7 +4079,7 @@
       </c>
       <c r="G96" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H96" t="n">
@@ -4117,7 +4117,7 @@
       </c>
       <c r="G97" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H97" t="n">
@@ -4155,7 +4155,7 @@
       </c>
       <c r="G98" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H98" t="n">
@@ -4193,7 +4193,7 @@
       </c>
       <c r="G99" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H99" t="n">
@@ -4231,7 +4231,7 @@
       </c>
       <c r="G100" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H100" t="n">
@@ -4269,7 +4269,7 @@
       </c>
       <c r="G101" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H101" t="n">
@@ -4307,7 +4307,7 @@
       </c>
       <c r="G102" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H102" t="n">
@@ -4345,7 +4345,7 @@
       </c>
       <c r="G103" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H103" t="n">
@@ -4383,7 +4383,7 @@
       </c>
       <c r="G104" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H104" t="n">
@@ -4421,7 +4421,7 @@
       </c>
       <c r="G105" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H105" t="n">
@@ -4459,7 +4459,7 @@
       </c>
       <c r="G106" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H106" t="n">
@@ -4497,7 +4497,7 @@
       </c>
       <c r="G107" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H107" t="n">
@@ -4535,7 +4535,7 @@
       </c>
       <c r="G108" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H108" t="n">
@@ -4573,7 +4573,7 @@
       </c>
       <c r="G109" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H109" t="n">
@@ -4611,7 +4611,7 @@
       </c>
       <c r="G110" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H110" t="n">
@@ -4649,7 +4649,7 @@
       </c>
       <c r="G111" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H111" t="n">
@@ -4687,7 +4687,7 @@
       </c>
       <c r="G112" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H112" t="n">
@@ -4725,7 +4725,7 @@
       </c>
       <c r="G113" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H113" t="n">
@@ -4763,7 +4763,7 @@
       </c>
       <c r="G114" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H114" t="n">
@@ -4801,7 +4801,7 @@
       </c>
       <c r="G115" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H115" t="n">
@@ -4839,7 +4839,7 @@
       </c>
       <c r="G116" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H116" t="n">
@@ -4877,7 +4877,7 @@
       </c>
       <c r="G117" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H117" t="n">
@@ -4915,7 +4915,7 @@
       </c>
       <c r="G118" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H118" t="n">
@@ -4953,7 +4953,7 @@
       </c>
       <c r="G119" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H119" t="n">
@@ -4991,7 +4991,7 @@
       </c>
       <c r="G120" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H120" t="n">
@@ -5029,7 +5029,7 @@
       </c>
       <c r="G121" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H121" t="n">
@@ -5067,7 +5067,7 @@
       </c>
       <c r="G122" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H122" t="n">
@@ -5105,7 +5105,7 @@
       </c>
       <c r="G123" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H123" t="n">
@@ -5143,7 +5143,7 @@
       </c>
       <c r="G124" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H124" t="n">
@@ -5181,7 +5181,7 @@
       </c>
       <c r="G125" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H125" t="n">
@@ -5219,7 +5219,7 @@
       </c>
       <c r="G126" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H126" t="n">
@@ -5257,7 +5257,7 @@
       </c>
       <c r="G127" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H127" t="n">
@@ -5295,7 +5295,7 @@
       </c>
       <c r="G128" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H128" t="n">
@@ -5333,7 +5333,7 @@
       </c>
       <c r="G129" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H129" t="n">
@@ -5371,7 +5371,7 @@
       </c>
       <c r="G130" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H130" t="n">
@@ -5409,7 +5409,7 @@
       </c>
       <c r="G131" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H131" t="n">
@@ -5447,7 +5447,7 @@
       </c>
       <c r="G132" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H132" t="n">
@@ -5485,7 +5485,7 @@
       </c>
       <c r="G133" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H133" t="n">
@@ -5523,7 +5523,7 @@
       </c>
       <c r="G134" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H134" t="n">
@@ -5561,7 +5561,7 @@
       </c>
       <c r="G135" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H135" t="n">
@@ -5599,7 +5599,7 @@
       </c>
       <c r="G136" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H136" t="n">
@@ -5637,7 +5637,7 @@
       </c>
       <c r="G137" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H137" t="n">
@@ -5675,7 +5675,7 @@
       </c>
       <c r="G138" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H138" t="n">
@@ -5713,7 +5713,7 @@
       </c>
       <c r="G139" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H139" t="n">
@@ -5751,7 +5751,7 @@
       </c>
       <c r="G140" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H140" t="n">
@@ -5789,7 +5789,7 @@
       </c>
       <c r="G141" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H141" t="n">
@@ -5827,7 +5827,7 @@
       </c>
       <c r="G142" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H142" t="n">
@@ -5865,7 +5865,7 @@
       </c>
       <c r="G143" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H143" t="n">
@@ -5903,7 +5903,7 @@
       </c>
       <c r="G144" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H144" t="n">
@@ -5941,7 +5941,7 @@
       </c>
       <c r="G145" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H145" t="n">
@@ -5979,7 +5979,7 @@
       </c>
       <c r="G146" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H146" t="n">
@@ -6017,7 +6017,7 @@
       </c>
       <c r="G147" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H147" t="n">
@@ -6055,7 +6055,7 @@
       </c>
       <c r="G148" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H148" t="n">
@@ -6093,7 +6093,7 @@
       </c>
       <c r="G149" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H149" t="n">
@@ -6131,7 +6131,7 @@
       </c>
       <c r="G150" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H150" t="n">
@@ -6169,7 +6169,7 @@
       </c>
       <c r="G151" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H151" t="n">
@@ -6207,7 +6207,7 @@
       </c>
       <c r="G152" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H152" t="n">
@@ -6245,7 +6245,7 @@
       </c>
       <c r="G153" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H153" t="n">
@@ -6283,7 +6283,7 @@
       </c>
       <c r="G154" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H154" t="n">
@@ -6321,7 +6321,7 @@
       </c>
       <c r="G155" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H155" t="n">
@@ -6359,7 +6359,7 @@
       </c>
       <c r="G156" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H156" t="n">
@@ -6397,7 +6397,7 @@
       </c>
       <c r="G157" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H157" t="n">
@@ -6435,7 +6435,7 @@
       </c>
       <c r="G158" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H158" t="n">
@@ -6473,7 +6473,7 @@
       </c>
       <c r="G159" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H159" t="n">
@@ -6511,7 +6511,7 @@
       </c>
       <c r="G160" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H160" t="n">
@@ -6549,7 +6549,7 @@
       </c>
       <c r="G161" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H161" t="n">
@@ -6587,7 +6587,7 @@
       </c>
       <c r="G162" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H162" t="n">
@@ -6625,7 +6625,7 @@
       </c>
       <c r="G163" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H163" t="n">
@@ -6663,7 +6663,7 @@
       </c>
       <c r="G164" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H164" t="n">
@@ -6701,7 +6701,7 @@
       </c>
       <c r="G165" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H165" t="n">
@@ -6739,7 +6739,7 @@
       </c>
       <c r="G166" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H166" t="n">
@@ -6777,7 +6777,7 @@
       </c>
       <c r="G167" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H167" t="n">
@@ -6815,7 +6815,7 @@
       </c>
       <c r="G168" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H168" t="n">
@@ -6853,7 +6853,7 @@
       </c>
       <c r="G169" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H169" t="n">
@@ -6891,7 +6891,7 @@
       </c>
       <c r="G170" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H170" t="n">
@@ -6929,7 +6929,7 @@
       </c>
       <c r="G171" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H171" t="n">
@@ -6967,7 +6967,7 @@
       </c>
       <c r="G172" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H172" t="n">
@@ -7005,7 +7005,7 @@
       </c>
       <c r="G173" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H173" t="n">
@@ -7043,7 +7043,7 @@
       </c>
       <c r="G174" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H174" t="n">
@@ -7081,7 +7081,7 @@
       </c>
       <c r="G175" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H175" t="n">
@@ -7119,7 +7119,7 @@
       </c>
       <c r="G176" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H176" t="n">
@@ -7157,7 +7157,7 @@
       </c>
       <c r="G177" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H177" t="n">
@@ -7195,7 +7195,7 @@
       </c>
       <c r="G178" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H178" t="n">
@@ -7233,7 +7233,7 @@
       </c>
       <c r="G179" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H179" t="n">
@@ -7271,7 +7271,7 @@
       </c>
       <c r="G180" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H180" t="n">
@@ -7309,7 +7309,7 @@
       </c>
       <c r="G181" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H181" t="n">
@@ -7347,7 +7347,7 @@
       </c>
       <c r="G182" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H182" t="n">
@@ -7385,7 +7385,7 @@
       </c>
       <c r="G183" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H183" t="n">
@@ -7423,7 +7423,7 @@
       </c>
       <c r="G184" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H184" t="n">
@@ -7461,7 +7461,7 @@
       </c>
       <c r="G185" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H185" t="n">
@@ -7499,7 +7499,7 @@
       </c>
       <c r="G186" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H186" t="n">
@@ -7537,7 +7537,7 @@
       </c>
       <c r="G187" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H187" t="n">
@@ -7575,7 +7575,7 @@
       </c>
       <c r="G188" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H188" t="n">
@@ -7613,7 +7613,7 @@
       </c>
       <c r="G189" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H189" t="n">
@@ -7651,7 +7651,7 @@
       </c>
       <c r="G190" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H190" t="n">
@@ -7689,7 +7689,7 @@
       </c>
       <c r="G191" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H191" t="n">
@@ -7727,7 +7727,7 @@
       </c>
       <c r="G192" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H192" t="n">
@@ -7765,7 +7765,7 @@
       </c>
       <c r="G193" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H193" t="n">
@@ -7803,7 +7803,7 @@
       </c>
       <c r="G194" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H194" t="n">
@@ -7841,7 +7841,7 @@
       </c>
       <c r="G195" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H195" t="n">
@@ -7879,7 +7879,7 @@
       </c>
       <c r="G196" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H196" t="n">
@@ -7917,7 +7917,7 @@
       </c>
       <c r="G197" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H197" t="n">
@@ -7955,7 +7955,7 @@
       </c>
       <c r="G198" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H198" t="n">
@@ -7993,7 +7993,7 @@
       </c>
       <c r="G199" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H199" t="n">
@@ -8031,7 +8031,7 @@
       </c>
       <c r="G200" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H200" t="n">
@@ -8069,7 +8069,7 @@
       </c>
       <c r="G201" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H201" t="n">
@@ -8107,7 +8107,7 @@
       </c>
       <c r="G202" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H202" t="n">
@@ -8145,7 +8145,7 @@
       </c>
       <c r="G203" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H203" t="n">
@@ -8183,7 +8183,7 @@
       </c>
       <c r="G204" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H204" t="n">
@@ -8221,7 +8221,7 @@
       </c>
       <c r="G205" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H205" t="n">
@@ -8259,7 +8259,7 @@
       </c>
       <c r="G206" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H206" t="n">
@@ -8297,7 +8297,7 @@
       </c>
       <c r="G207" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H207" t="n">
@@ -8335,7 +8335,7 @@
       </c>
       <c r="G208" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H208" t="n">
@@ -8373,7 +8373,7 @@
       </c>
       <c r="G209" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H209" t="n">
@@ -8411,7 +8411,7 @@
       </c>
       <c r="G210" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H210" t="n">
@@ -8449,7 +8449,7 @@
       </c>
       <c r="G211" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H211" t="n">
@@ -8487,7 +8487,7 @@
       </c>
       <c r="G212" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H212" t="n">
@@ -8525,7 +8525,7 @@
       </c>
       <c r="G213" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H213" t="n">
@@ -8563,7 +8563,7 @@
       </c>
       <c r="G214" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H214" t="n">
@@ -8601,7 +8601,7 @@
       </c>
       <c r="G215" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H215" t="n">
@@ -8639,7 +8639,7 @@
       </c>
       <c r="G216" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H216" t="n">
@@ -8677,7 +8677,7 @@
       </c>
       <c r="G217" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H217" t="n">
@@ -8715,7 +8715,7 @@
       </c>
       <c r="G218" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H218" t="n">
@@ -8753,7 +8753,7 @@
       </c>
       <c r="G219" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H219" t="n">
@@ -8791,7 +8791,7 @@
       </c>
       <c r="G220" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H220" t="n">
@@ -8829,7 +8829,7 @@
       </c>
       <c r="G221" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H221" t="n">
@@ -8867,7 +8867,7 @@
       </c>
       <c r="G222" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H222" t="n">
@@ -8905,7 +8905,7 @@
       </c>
       <c r="G223" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H223" t="n">
@@ -8943,7 +8943,7 @@
       </c>
       <c r="G224" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H224" t="n">
@@ -8981,7 +8981,7 @@
       </c>
       <c r="G225" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H225" t="n">
@@ -9019,7 +9019,7 @@
       </c>
       <c r="G226" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H226" t="n">
@@ -9057,7 +9057,7 @@
       </c>
       <c r="G227" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H227" t="n">
@@ -9095,7 +9095,7 @@
       </c>
       <c r="G228" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H228" t="n">
@@ -9133,7 +9133,7 @@
       </c>
       <c r="G229" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H229" t="n">
@@ -9171,7 +9171,7 @@
       </c>
       <c r="G230" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H230" t="n">
@@ -9209,7 +9209,7 @@
       </c>
       <c r="G231" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H231" t="n">
@@ -9247,7 +9247,7 @@
       </c>
       <c r="G232" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H232" t="n">
@@ -9285,7 +9285,7 @@
       </c>
       <c r="G233" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H233" t="n">
@@ -9323,7 +9323,7 @@
       </c>
       <c r="G234" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H234" t="n">
@@ -9361,7 +9361,7 @@
       </c>
       <c r="G235" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H235" t="n">
@@ -9399,7 +9399,7 @@
       </c>
       <c r="G236" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H236" t="n">
@@ -9437,7 +9437,7 @@
       </c>
       <c r="G237" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H237" t="n">
@@ -9475,7 +9475,7 @@
       </c>
       <c r="G238" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H238" t="n">
@@ -9513,7 +9513,7 @@
       </c>
       <c r="G239" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H239" t="n">
@@ -9551,7 +9551,7 @@
       </c>
       <c r="G240" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H240" t="n">
@@ -9589,7 +9589,7 @@
       </c>
       <c r="G241" t="inlineStr">
         <is>
-          <t>2025-08-29T08:32:47Z</t>
+          <t>2025-08-29T10:17:02Z</t>
         </is>
       </c>
       <c r="H241" t="n">

</xml_diff>